<commit_message>
added Global Tasks for final Release
</commit_message>
<xml_diff>
--- a/Planning/Planning_2_5_9_5.xlsx
+++ b/Planning/Planning_2_5_9_5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09EAC97-62CE-44A3-BD20-11945BDD7E9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177DF9BA-B7F3-4EA7-8E76-F139778F1513}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,7 +379,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated Planníng KW 18
</commit_message>
<xml_diff>
--- a/Planning/Planning_2_5_9_5.xlsx
+++ b/Planning/Planning_2_5_9_5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D25C7D-917D-46A6-914C-22233B048DC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98945586-CA2E-41A0-A19D-77D9924C44D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Task</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>Coin Flip against User</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,10 +428,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -458,8 +461,28 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>